<commit_message>
add passive unit type & max 3 melee attacks
</commit_message>
<xml_diff>
--- a/contents/battle/battle_7/battle_7.xlsx
+++ b/contents/battle/battle_7/battle_7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imanol-KS53\Documents\Imanol\Github_projects\InteractiveBook\contents\battle\battle_7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE7F3CA-5DC3-42D2-8028-8320EF7DB516}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAC94E65-B3A3-4500-9153-2F70DB640572}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="9885" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nodes" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="56">
   <si>
     <t>x</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Caravan</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -582,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="F107" sqref="F107"/>
+    <sheetView topLeftCell="A75" workbookViewId="0">
+      <selection activeCell="I90" sqref="I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,7 +1532,9 @@
       <c r="E49" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F49" s="5"/>
+      <c r="F49" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G49" s="5"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -1548,7 +1553,9 @@
       <c r="E50" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F50" s="5"/>
+      <c r="F50" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G50" s="5"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -1567,7 +1574,9 @@
       <c r="E51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="5"/>
+      <c r="F51" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G51" s="5"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -1586,7 +1595,9 @@
       <c r="E52" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F52" s="5"/>
+      <c r="F52" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G52" s="5"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,7 +1616,9 @@
       <c r="E53" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F53" s="5"/>
+      <c r="F53" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G53" s="5"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -1624,7 +1637,9 @@
       <c r="E54" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F54" s="5"/>
+      <c r="F54" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G54" s="5"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -1643,7 +1658,9 @@
       <c r="E55" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F55" s="5"/>
+      <c r="F55" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G55" s="5"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -1662,7 +1679,9 @@
       <c r="E56" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F56" s="5"/>
+      <c r="F56" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G56" s="5"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -1681,7 +1700,9 @@
       <c r="E57" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F57" s="5"/>
+      <c r="F57" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G57" s="5"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -1700,7 +1721,9 @@
       <c r="E58" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="F58" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G58" s="12" t="s">
         <v>53</v>
       </c>
@@ -1742,7 +1765,9 @@
       <c r="E60" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F60" s="5"/>
+      <c r="F60" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G60" s="12" t="s">
         <v>53</v>
       </c>
@@ -1763,7 +1788,9 @@
       <c r="E61" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F61" s="5"/>
+      <c r="F61" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G61" s="5"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -1782,7 +1809,9 @@
       <c r="E62" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F62" s="5"/>
+      <c r="F62" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G62" s="5"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -1801,7 +1830,9 @@
       <c r="E63" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F63" s="5"/>
+      <c r="F63" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G63" s="5"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -1820,7 +1851,9 @@
       <c r="E64" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F64" s="5"/>
+      <c r="F64" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G64" s="5"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -1839,7 +1872,9 @@
       <c r="E65" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F65" s="5"/>
+      <c r="F65" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G65" s="5"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -1858,7 +1893,9 @@
       <c r="E66" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F66" s="5"/>
+      <c r="F66" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G66" s="5"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -1877,7 +1914,9 @@
       <c r="E67" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F67" s="5"/>
+      <c r="F67" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G67" s="5"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -1896,7 +1935,9 @@
       <c r="E68" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F68" s="5"/>
+      <c r="F68" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G68" s="5"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -1915,7 +1956,9 @@
       <c r="E69" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F69" s="5"/>
+      <c r="F69" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G69" s="5"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -1934,7 +1977,9 @@
       <c r="E70" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F70" s="5"/>
+      <c r="F70" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G70" s="5"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -1953,7 +1998,9 @@
       <c r="E71" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F71" s="5"/>
+      <c r="F71" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G71" s="5"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -1972,7 +2019,9 @@
       <c r="E72" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F72" s="5"/>
+      <c r="F72" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G72" s="5"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -1991,7 +2040,9 @@
       <c r="E73" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F73" s="5"/>
+      <c r="F73" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G73" s="5"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -2010,7 +2061,9 @@
       <c r="E74" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F74" s="5"/>
+      <c r="F74" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G74" s="5"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -2029,7 +2082,9 @@
       <c r="E75" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F75" s="5"/>
+      <c r="F75" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G75" s="5"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -2048,7 +2103,9 @@
       <c r="E76" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F76" s="5"/>
+      <c r="F76" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G76" s="5"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -2067,7 +2124,9 @@
       <c r="E77" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F77" s="5"/>
+      <c r="F77" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -2086,7 +2145,9 @@
       <c r="E78" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F78" s="5"/>
+      <c r="F78" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G78" s="12" t="s">
         <v>53</v>
       </c>
@@ -2107,7 +2168,9 @@
       <c r="E79" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F79" s="5"/>
+      <c r="F79" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G79" s="12" t="s">
         <v>53</v>
       </c>
@@ -2128,7 +2191,9 @@
       <c r="E80" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F80" s="5"/>
+      <c r="F80" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G80" s="5"/>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -2147,7 +2212,9 @@
       <c r="E81" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F81" s="5"/>
+      <c r="F81" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G81" s="5"/>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -2166,7 +2233,9 @@
       <c r="E82" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F82" s="5"/>
+      <c r="F82" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G82" s="5"/>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -2185,7 +2254,9 @@
       <c r="E83" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F83" s="5"/>
+      <c r="F83" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G83" s="5"/>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -2204,7 +2275,9 @@
       <c r="E84" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F84" s="5"/>
+      <c r="F84" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G84" s="5"/>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -2223,7 +2296,9 @@
       <c r="E85" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F85" s="5"/>
+      <c r="F85" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G85" s="5"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -2242,7 +2317,9 @@
       <c r="E86" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F86" s="5"/>
+      <c r="F86" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G86" s="5"/>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,7 +2338,9 @@
       <c r="E87" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F87" s="5"/>
+      <c r="F87" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G87" s="5"/>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -2280,7 +2359,9 @@
       <c r="E88" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F88" s="5"/>
+      <c r="F88" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G88" s="5"/>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -2299,7 +2380,9 @@
       <c r="E89" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F89" s="5"/>
+      <c r="F89" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G89" s="5"/>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -2318,7 +2401,9 @@
       <c r="E90" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F90" s="5"/>
+      <c r="F90" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G90" s="5"/>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -2337,7 +2422,9 @@
       <c r="E91" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F91" s="5"/>
+      <c r="F91" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G91" s="5"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -2356,7 +2443,9 @@
       <c r="E92" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F92" s="5"/>
+      <c r="F92" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G92" s="5"/>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -2375,7 +2464,9 @@
       <c r="E93" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F93" s="5"/>
+      <c r="F93" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G93" s="5"/>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -2394,7 +2485,9 @@
       <c r="E94" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F94" s="5"/>
+      <c r="F94" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="G94" s="12" t="s">
         <v>53</v>
       </c>
@@ -2415,7 +2508,9 @@
       <c r="E95" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F95" s="5"/>
+      <c r="F95" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G95" s="12" t="s">
         <v>53</v>
       </c>
@@ -2436,7 +2531,9 @@
       <c r="E96" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F96" s="5"/>
+      <c r="F96" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G96" s="5"/>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2455,7 +2552,9 @@
       <c r="E97" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F97" s="5"/>
+      <c r="F97" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G97" s="5"/>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -2474,7 +2573,9 @@
       <c r="E98" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F98" s="5"/>
+      <c r="F98" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G98" s="5"/>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -2493,7 +2594,9 @@
       <c r="E99" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F99" s="5"/>
+      <c r="F99" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G99" s="5"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -2512,7 +2615,9 @@
       <c r="E100" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F100" s="5"/>
+      <c r="F100" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G100" s="5"/>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -2531,7 +2636,9 @@
       <c r="E101" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F101" s="5"/>
+      <c r="F101" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G101" s="5"/>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -2550,7 +2657,9 @@
       <c r="E102" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F102" s="5"/>
+      <c r="F102" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G102" s="5"/>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -2569,7 +2678,9 @@
       <c r="E103" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F103" s="5"/>
+      <c r="F103" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G103" s="5"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -2588,7 +2699,9 @@
       <c r="E104" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F104" s="5"/>
+      <c r="F104" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G104" s="5"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -2607,7 +2720,9 @@
       <c r="E105" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F105" s="5"/>
+      <c r="F105" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G105" s="5"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -2626,7 +2741,9 @@
       <c r="E106" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F106" s="5"/>
+      <c r="F106" s="6" t="s">
+        <v>52</v>
+      </c>
       <c r="G106" s="5"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -3699,8 +3816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B76CDC32-9C71-4924-88B2-6E23C700FAA0}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3759,7 +3876,7 @@
   <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4587,7 +4704,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E24" s="8">
         <v>0</v>
@@ -4622,7 +4739,7 @@
         <v>54</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E25" s="8">
         <v>0</v>
@@ -4657,7 +4774,7 @@
         <v>54</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="E26" s="8">
         <v>0</v>
@@ -4847,7 +4964,7 @@
         <v>7</v>
       </c>
       <c r="I31" s="1">
-        <v>151</v>
+        <v>64</v>
       </c>
       <c r="J31" s="8">
         <v>1</v>

</xml_diff>